<commit_message>
2) inicios de sesion en un periodo de tiempo determinado, terminado
</commit_message>
<xml_diff>
--- a/TP_FINAL/Conexiones de usuario.xlsx
+++ b/TP_FINAL/Conexiones de usuario.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:D1"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,18 +440,338 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Usuario</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Inicio de Conexi¢n</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Fin de Conexio</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Usuario</t>
-        </is>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>43705.42083333333</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>43705.42083333333</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>43705.42083333333</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>43705.42152777778</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>43705.42152777778</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>43705.42152777778</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>43705.42152777778</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>43705.42152777778</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>43705.42361111111</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>43705.42361111111</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>43705.42361111111</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>43705.42361111111</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>43705.42361111111</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>43705.42361111111</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>43705.42430555556</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>43705.42430555556</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>43705.42430555556</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>43705.42430555556</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>43705.42430555556</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>43705.425</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>43705.42569444444</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>43705.42638888889</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>43705.42638888889</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>43705.42708333334</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>invitede-pansew</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>43705.42777777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>